<commit_message>
last day on the job
</commit_message>
<xml_diff>
--- a/Literature/Lit_Review_Summaries.xlsx
+++ b/Literature/Lit_Review_Summaries.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/.shortcut-targets-by-id/0B0efpUDNVRiVME9hOFNHaU1xVW8/Nutrition_BiasInScience/Literature/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D65A1A-A133-214D-8762-B5A065D45816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15440" xr2:uid="{D899292F-DD4A-5641-98A6-382254214528}"/>
+    <workbookView xWindow="465" yWindow="465" windowWidth="27645" windowHeight="15435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>Article Title</t>
   </si>
@@ -118,13 +113,241 @@
   <si>
     <t>Supportive authors were significantly more likely than critical or neutral authors to have financial relationships with P&amp;G (80% vs 11% and 21%, respectively;
 P&lt;.0001). All authors disclosing an affiliation with P&amp;G were supportive.</t>
+  </si>
+  <si>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t>Journal of Publication</t>
+  </si>
+  <si>
+    <t>Academic Field</t>
+  </si>
+  <si>
+    <t>PLOS Medicine</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Different groups of investigators handcoded either financial sponsors or article conclusions</t>
+  </si>
+  <si>
+    <t>Meta-analysis</t>
+  </si>
+  <si>
+    <t>JAMA Internal Medicine</t>
+  </si>
+  <si>
+    <t>Clinical Nutrition</t>
+  </si>
+  <si>
+    <t>Handcoded methodologic quality of reviews by independent reviewers</t>
+  </si>
+  <si>
+    <t>American Journal of Clinical Nutrition</t>
+  </si>
+  <si>
+    <t>Narrative case study of sugar industry internal documents</t>
+  </si>
+  <si>
+    <t>Handcoded by authors</t>
+  </si>
+  <si>
+    <t>International Journal of Obesity</t>
+  </si>
+  <si>
+    <t>Narrative approach</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Handcoded by authors and subject authors surveyed regarding financial relationships</t>
+  </si>
+  <si>
+    <t>American Journal of Public Health</t>
+  </si>
+  <si>
+    <t>Public Health</t>
+  </si>
+  <si>
+    <t>Association between industry funding
+and statistically significant pro-industry findings
+in medical and surgical randomized trials</t>
+  </si>
+  <si>
+    <t>Bhandari et al</t>
+  </si>
+  <si>
+    <t>Industry funding found to be associated with a statistically significant result in favor of new industry product, for medical trials and surgical interventions.</t>
+  </si>
+  <si>
+    <t>Canadian Medical Associatin Journal</t>
+  </si>
+  <si>
+    <t>Pharmaceutical industry sponsorship and research
+outcome and quality: systematic review</t>
+  </si>
+  <si>
+    <t>Lexchin et al</t>
+  </si>
+  <si>
+    <t>The BMJ</t>
+  </si>
+  <si>
+    <t>Studies sponsored by pharmaceutical companies were more likely to have outcomes favoring sponsor (95% CI: 2.98 - 5.51 OR)</t>
+  </si>
+  <si>
+    <t>Systematic review of 30 studies looking at research sponsored by pharmaceutical companies</t>
+  </si>
+  <si>
+    <t>Research grants, sources of ideas and the effects
+on academic research</t>
+  </si>
+  <si>
+    <t>Hottenrott and Lawson</t>
+  </si>
+  <si>
+    <t>Economics of Innovation and New Technology</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Survey data of research units in German higher education institutions. Publications and patent data manually matched.</t>
+  </si>
+  <si>
+    <t>The higher the share of industry funding in a research unit's budget, the greater role the firm has in the idea generation process. Industry funding is also associated with lower publication rates and lower impact on future work.</t>
+  </si>
+  <si>
+    <t>Pharmaceutical company funding and its consequences: A qualitative systematic review</t>
+  </si>
+  <si>
+    <t>Sismondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 out of 19 papers published from 2003-2006 show strong association between industry funding and pro-industry results. Earlier systematic reviews show 20 out of 23 with same effect. </t>
+  </si>
+  <si>
+    <t>Qualitative systematic review.</t>
+  </si>
+  <si>
+    <t>Contemporary Clinical Trials</t>
+  </si>
+  <si>
+    <t>Expertise versus Bias in in Evaluation: Evidence from the NIH</t>
+  </si>
+  <si>
+    <t>Danielle Li</t>
+  </si>
+  <si>
+    <t>Intellectual related reviewers increase grant applicant's chance of funding by 2.2%. High quality applicants benefit significantly more from being reviewed by biased experts than low quality applicants.</t>
+  </si>
+  <si>
+    <t>Dataset constructed using NIH administrative data. Measurements empirically constructed and causal analysis done using regression.</t>
+  </si>
+  <si>
+    <t>American Economic Journal: Applied Economics</t>
+  </si>
+  <si>
+    <t>Does Conflict of Interest Lead to Biased Coverage? Evidence from Movie Reviews</t>
+  </si>
+  <si>
+    <t>Dellavigna and Hermle</t>
+  </si>
+  <si>
+    <t>No evidence of bias in movie reviews by conglomerate-owned media outlets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movies clustered by genre and differences-in-differences approach to estimating bias. </t>
+  </si>
+  <si>
+    <t>Review of Economic Studies</t>
+  </si>
+  <si>
+    <t>Bias in published cost effectiveness studies: systematic review</t>
+  </si>
+  <si>
+    <t>Bell et al</t>
+  </si>
+  <si>
+    <t>Industry funded studies more likely to report cost effectiveness ratios below the standard cutoff thresholds. Studies with higher methodological quality were less likely to report ratios below $20k/QALY</t>
+  </si>
+  <si>
+    <t>Two independent reviewers manually evaluated each study. 95% CI odds ratios were computed.</t>
+  </si>
+  <si>
+    <t>Biases in fiscal multiplier estimates</t>
+  </si>
+  <si>
+    <t>Asatryan et al</t>
+  </si>
+  <si>
+    <t>Author characteristics manually coded from CVs and surveys. Meta-analytical regression analysis.</t>
+  </si>
+  <si>
+    <t>European Journal of Political Economy</t>
+  </si>
+  <si>
+    <t>National background and policy orientation significantly influence fiscal multiplier estimates. Some evidence of funding bias through national funding agencies and private institutions correlated with higher/lower multiplier estimates, respectively.</t>
+  </si>
+  <si>
+    <t>Factors Associated with Findings of Published
+Trials of Drug–Drug Comparisons: Why Some
+Statins Appear More Efficacious than Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bero et al </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCTs comparing statins with other drugs likely to report results favoring the sponsor's product. </t>
+  </si>
+  <si>
+    <t>Study details, author financial ties, and author conclusions manually extracted by two coders. Analysis: multivariate logistic regression</t>
+  </si>
+  <si>
+    <t>PlOS Medicine</t>
+  </si>
+  <si>
+    <t>Lundh et al</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry Sponsorship and Research Outcome </t>
+  </si>
+  <si>
+    <t>Significant association found between sponsorship of drug and device studies by manufacturing company and favorable efficacy results.</t>
+  </si>
+  <si>
+    <t>Independent investigators screened abstracts and extracted data. Sources: MEDLINE, Cochrane Registrar, Web of Science</t>
+  </si>
+  <si>
+    <t>Cochrane Database of Systematic Reviews</t>
+  </si>
+  <si>
+    <r>
+      <t>Industry-funded research finds 0% unfavorable conclusions compared to 37% for non-industry funded articles in soft-drink, juice and milk  (Lesser et all 2007), causal relation between SSB and weight gain was weak only in industry-funded research (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Massougbodji et al 2014), sugar shifts blame to fat (Kearns et al 2016 cited by the NY times article?), fat susbtiture olestra was supported more by authors with financial relationships with P&amp;G (Levine et al 2003)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Has been shown to exist in pharmaceutical research (meta analysiz Bekelman et al 2003) and nutrition research </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,13 +355,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,13 +401,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,31 +733,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6A2E90-D13F-9C40-92CF-615C7FD41204}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="55.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="55.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,8 +776,17 @@
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -521,8 +799,17 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -535,8 +822,17 @@
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -549,8 +845,17 @@
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -566,8 +871,17 @@
       <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -580,8 +894,17 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -597,8 +920,17 @@
       <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -610,9 +942,277 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2004</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2003</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2017</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2017</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2006</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2020</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>